<commit_message>
nivel 3 - practica 1
</commit_message>
<xml_diff>
--- a/Nivel 3/Practica 1/ReFramework_UiDemo/UiPath_REFrameWork_UiDemo/Data/Config.xlsx
+++ b/Nivel 3/Practica 1/ReFramework_UiDemo/UiPath_REFrameWork_UiDemo/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -155,15 +155,6 @@
     <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
   </si>
   <si>
-    <t>UiDemoCredential_REFramework</t>
-  </si>
-  <si>
-    <t>REFramework_UiDemo</t>
-  </si>
-  <si>
-    <t>QueueName</t>
-  </si>
-  <si>
     <t>Credencial used to log in to UiDemo</t>
   </si>
   <si>
@@ -174,6 +165,27 @@
   </si>
   <si>
     <t>Path to application UiDemo</t>
+  </si>
+  <si>
+    <t>logF_BusinessProcessName</t>
+  </si>
+  <si>
+    <t>Framework</t>
+  </si>
+  <si>
+    <t>SHA1OnlineURL</t>
+  </si>
+  <si>
+    <t>http://www.sha1-online.com/</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>Queue_REFramework_UiDemo</t>
+  </si>
+  <si>
+    <t>Credential_REFramework_UiDemo</t>
   </si>
 </sst>
 </file>
@@ -499,7 +511,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -546,10 +558,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
         <v>43</v>
@@ -557,17 +569,31 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>48</v>
       </c>
-      <c r="B3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" t="s">
-        <v>47</v>
+      <c r="B4" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2827,13 +2853,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>